<commit_message>
Added more test data to the file
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Eclipse Workspace\FreeCRMTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Eclipse Workspace\AmazonPOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D76D2AED-4E01-4475-909C-48120EC3D76F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1E4E1C-D6B6-43BD-B7AE-245DA8445F0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="2880" windowWidth="14400" windowHeight="7460" xr2:uid="{255D47C7-491B-4B33-9052-56195D9C7A92}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{255D47C7-491B-4B33-9052-56195D9C7A92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,24 +42,6 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Test4</t>
-  </si>
-  <si>
-    <t>Test5</t>
-  </si>
-  <si>
-    <t>IND1</t>
-  </si>
-  <si>
     <t>IND2</t>
   </si>
   <si>
@@ -70,6 +52,24 @@
   </si>
   <si>
     <t>IND5</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Raghu</t>
+  </si>
+  <si>
+    <t>Ashish</t>
   </si>
 </sst>
 </file>
@@ -430,10 +430,13 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -451,10 +454,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -462,10 +465,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -473,10 +476,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -484,10 +487,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -495,10 +498,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>